<commit_message>
xcel report for earnings and income
</commit_message>
<xml_diff>
--- a/src/report.xlsx
+++ b/src/report.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="IncomeReport" sheetId="1" r:id="rId1"/>
+    <sheet name="EarningsReport" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Revenue</t>
   </si>
@@ -53,6 +54,36 @@
   </si>
   <si>
     <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
+  </si>
+  <si>
+    <t>EPS Estimate</t>
+  </si>
+  <si>
+    <t>EPS Actual</t>
+  </si>
+  <si>
+    <t>EPS Surprise</t>
+  </si>
+  <si>
+    <t>EPS Growth Quarter and Year Forecast</t>
+  </si>
+  <si>
+    <t>Revenue Growth Quarter and Year Forecast</t>
+  </si>
+  <si>
+    <t>Price Delta</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>55900, 402</t>
+  </si>
+  <si>
+    <t>35, 35</t>
   </si>
 </sst>
 </file>
@@ -487,4 +518,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="2">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix xcel header names
</commit_message>
<xml_diff>
--- a/src/report.xlsx
+++ b/src/report.xlsx
@@ -23,19 +23,19 @@
     <t>Revenue</t>
   </si>
   <si>
-    <t>Rev. Growth</t>
+    <t>Rev. Growth (%)</t>
   </si>
   <si>
     <t>Earnings</t>
   </si>
   <si>
-    <t>EPS Growth</t>
+    <t>EPS Growth (%)</t>
   </si>
   <si>
     <t>FCF</t>
   </si>
   <si>
-    <t>FCF Growth</t>
+    <t>FCF Growth (%)</t>
   </si>
   <si>
     <t>Price/Earnings/Growth</t>
@@ -68,13 +68,13 @@
     <t>EPS Actual</t>
   </si>
   <si>
-    <t>EPS Surprise</t>
-  </si>
-  <si>
-    <t>EPS Growth Quarter and Year Forecast</t>
-  </si>
-  <si>
-    <t>Revenue Growth Quarter and Year Forecast</t>
+    <t>EPS Surprise (%)</t>
+  </si>
+  <si>
+    <t>EPS Growth Quarter and Year Forecast (%)</t>
+  </si>
+  <si>
+    <t>Revenue Growth Quarter and Year Forecast (%)</t>
   </si>
   <si>
     <t>Price Delta</t>
@@ -461,11 +461,11 @@
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
@@ -544,9 +544,9 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
process eps for earnings obj
</commit_message>
<xml_diff>
--- a/src/report.xlsx
+++ b/src/report.xlsx
@@ -44,22 +44,22 @@
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>CRWD</t>
-  </si>
-  <si>
-    <t>487.83M -&gt; 535.15M -&gt; 580.88M -&gt; 637.37M -&gt; 692.58M</t>
-  </si>
-  <si>
-    <t>-0.14 -&gt; -0.21 -&gt; -0.24 -&gt; -0.2 -&gt; 0.0</t>
-  </si>
-  <si>
-    <t>159.74M -&gt; 138.25M -&gt; 176.41M -&gt; 212.85M -&gt; 230.93M</t>
-  </si>
-  <si>
-    <t>1.61 &lt;- 1.22 &lt;- 2.19 &lt;- 3.79 &lt;- 4.63</t>
-  </si>
-  <si>
-    <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>495.78M -&gt; 584.58M -&gt; 631.91M -&gt; 609.15M -&gt; 589.85M</t>
+  </si>
+  <si>
+    <t>-0.42 -&gt; -0.06 -&gt; 0.96 -&gt; 0.29 -&gt; -1.12</t>
+  </si>
+  <si>
+    <t>(683.51M) -&gt; (716.05M) -&gt; (636.94M) -&gt; (823.36M) -&gt; (949.63M)</t>
+  </si>
+  <si>
+    <t>N/A &lt;- N/A &lt;- N/A &lt;- N/A</t>
+  </si>
+  <si>
+    <t>1.90 &lt;- 2.41 &lt;- 2.95 &lt;- 2.73</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -80,16 +80,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>55900, 402</t>
-  </si>
-  <si>
-    <t>35, 35</t>
+    <t>-0.13</t>
+  </si>
+  <si>
+    <t>-1.12</t>
+  </si>
+  <si>
+    <t>83, -269</t>
+  </si>
+  <si>
+    <t>7, 8</t>
   </si>
 </sst>
 </file>
@@ -462,12 +462,12 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1">
@@ -507,19 +507,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>100</v>
+        <v>-167</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2">
-        <v>45</v>
+        <v>-39</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -584,7 +584,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>11</v>
+        <v>-761</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -593,7 +593,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="2">
-        <v>47</v>
+        <v>-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move data processing funcs to util
</commit_message>
<xml_diff>
--- a/src/report.xlsx
+++ b/src/report.xlsx
@@ -44,22 +44,22 @@
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>RUN</t>
-  </si>
-  <si>
-    <t>495.78M -&gt; 584.58M -&gt; 631.91M -&gt; 609.15M -&gt; 589.85M</t>
-  </si>
-  <si>
-    <t>-0.42 -&gt; -0.06 -&gt; 0.96 -&gt; 0.29 -&gt; -1.12</t>
-  </si>
-  <si>
-    <t>(683.51M) -&gt; (716.05M) -&gt; (636.94M) -&gt; (823.36M) -&gt; (949.63M)</t>
-  </si>
-  <si>
-    <t>N/A &lt;- N/A &lt;- N/A &lt;- N/A</t>
-  </si>
-  <si>
-    <t>1.90 &lt;- 2.41 &lt;- 2.95 &lt;- 2.73</t>
+    <t>CRWD</t>
+  </si>
+  <si>
+    <t>487.83M -&gt; 535.15M -&gt; 580.88M -&gt; 637.37M -&gt; 692.58M</t>
+  </si>
+  <si>
+    <t>-0.14 -&gt; -0.21 -&gt; -0.24 -&gt; -0.2 -&gt; 0.0</t>
+  </si>
+  <si>
+    <t>159.74M -&gt; 138.25M -&gt; 176.41M -&gt; 212.85M -&gt; 230.93M</t>
+  </si>
+  <si>
+    <t>1.61 &lt;- 1.22 &lt;- 2.19 &lt;- 3.79 &lt;- 4.63</t>
+  </si>
+  <si>
+    <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -80,16 +80,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>-0.13</t>
-  </si>
-  <si>
-    <t>-1.12</t>
-  </si>
-  <si>
-    <t>83, -269</t>
-  </si>
-  <si>
-    <t>7, 8</t>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>55900, 402</t>
+  </si>
+  <si>
+    <t>35, 35</t>
   </si>
 </sst>
 </file>
@@ -462,12 +462,12 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1">
@@ -507,19 +507,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>-167</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2">
-        <v>-39</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -584,7 +584,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>-761</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -593,7 +593,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="2">
-        <v>-13</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>